<commit_message>
Add new benchmark and ablation files for multicore testing
</commit_message>
<xml_diff>
--- a/ablation-revised/ablation.xlsx
+++ b/ablation-revised/ablation.xlsx
@@ -64,7 +64,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +81,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -112,37 +118,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -446,28 +461,29 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="34.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="44.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3" t="s">
@@ -476,29 +492,30 @@
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="3" t="s">
+      <c r="L1" s="4"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -506,164 +523,176 @@
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="7">
         <v>1</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="8">
         <v>1.046469666</v>
       </c>
-      <c r="D2" s="6">
-        <v>1.109121288</v>
-      </c>
-      <c r="E2" s="7">
-        <v>1.06277872</v>
-      </c>
-      <c r="F2" s="7">
-        <v>1.06853422</v>
-      </c>
-      <c r="G2" s="7">
+      <c r="D2" s="8">
+        <v>1.220290755</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1.088374371</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1.201244868</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1.065259394</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1.226602354</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.09786521</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1.193264524</v>
+      </c>
+      <c r="K2" s="3">
         <v>1.081262376</v>
       </c>
-      <c r="H2" s="7">
+      <c r="L2" s="3">
+        <v>1.393359136</v>
+      </c>
+      <c r="M2" s="9">
         <v>1.250514984</v>
       </c>
-      <c r="I2" s="7">
-        <v>1.248703238</v>
-      </c>
-      <c r="J2" s="7">
-        <v>1.202368759</v>
-      </c>
-      <c r="K2" s="7">
-        <v>1.210128105</v>
-      </c>
-      <c r="L2" s="7">
-        <v>1.221121667</v>
-      </c>
-      <c r="M2" s="6">
-        <v>1.393359136</v>
+      <c r="N2" s="8">
+        <v>1.410047258</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="7">
         <v>1</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="8">
         <v>1.044947754</v>
       </c>
-      <c r="D3" s="6">
-        <v>1.107706667</v>
-      </c>
-      <c r="E3" s="7">
-        <v>1.096956163</v>
-      </c>
-      <c r="F3" s="7">
-        <v>1.069144882</v>
-      </c>
-      <c r="G3" s="7">
+      <c r="D3" s="8">
+        <v>1.222614297</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.088441801</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1.201961981</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1.063494276</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1.223025188</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.097107283</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1.194124163</v>
+      </c>
+      <c r="K3" s="3">
         <v>1.080079914</v>
       </c>
-      <c r="H3" s="7">
+      <c r="L3" s="3">
+        <v>1.400666465</v>
+      </c>
+      <c r="M3" s="9">
         <v>1.258327406</v>
       </c>
-      <c r="I3" s="7">
-        <v>1.246094612</v>
-      </c>
-      <c r="J3" s="7">
-        <v>1.277988772</v>
-      </c>
-      <c r="K3" s="7">
-        <v>1.207891607</v>
-      </c>
-      <c r="L3" s="7">
-        <v>1.216981306</v>
-      </c>
-      <c r="M3" s="6">
-        <v>1.400666465</v>
+      <c r="N3" s="8">
+        <v>1.411655629</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="7">
         <v>1</v>
       </c>
-      <c r="C4" s="6">
-        <v>1.048715042</v>
-      </c>
-      <c r="D4" s="6">
+      <c r="C4" s="8">
+        <v>1.048338979</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1.195723665</v>
+      </c>
+      <c r="E4" s="3">
         <v>1.097846976</v>
       </c>
-      <c r="E4" s="7">
+      <c r="F4" s="3">
+        <v>1.158447513</v>
+      </c>
+      <c r="G4" s="3">
         <v>1.066200261</v>
       </c>
-      <c r="F4" s="7">
-        <v>1.057267739</v>
-      </c>
-      <c r="G4" s="7">
+      <c r="H4" s="3">
+        <v>1.161759297</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1.066450554</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1.179059897</v>
+      </c>
+      <c r="K4" s="3">
         <v>1.074580819</v>
       </c>
-      <c r="H4" s="7">
-        <v>1.250482724</v>
-      </c>
-      <c r="I4" s="7">
-        <v>1.195723665</v>
-      </c>
-      <c r="J4" s="7">
-        <v>1.158447513</v>
-      </c>
-      <c r="K4" s="7">
-        <v>1.161759297</v>
-      </c>
-      <c r="L4" s="7">
-        <v>1.179059897</v>
-      </c>
-      <c r="M4" s="6">
-        <v>1.367047725</v>
+      <c r="L4" s="3">
+        <v>1.366567845</v>
+      </c>
+      <c r="M4" s="9">
+        <v>1.257503414</v>
+      </c>
+      <c r="N4" s="8">
+        <v>1.440002459</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="7">
         <v>1</v>
       </c>
-      <c r="C5" s="6">
-        <v>1.056303854</v>
-      </c>
-      <c r="D5" s="6">
+      <c r="C5" s="8">
+        <v>1.045820092</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1.189579543</v>
+      </c>
+      <c r="E5" s="3">
         <v>1.101474491</v>
       </c>
-      <c r="E5" s="7">
+      <c r="F5" s="3">
+        <v>1.159648563</v>
+      </c>
+      <c r="G5" s="3">
         <v>1.071425026</v>
       </c>
-      <c r="F5" s="7">
-        <v>1.056874328</v>
-      </c>
-      <c r="G5" s="7">
+      <c r="H5" s="3">
+        <v>1.156311054</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1.064313615</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1.170361225</v>
+      </c>
+      <c r="K5" s="3">
         <v>1.076043693</v>
       </c>
-      <c r="H5" s="7">
-        <v>1.303616355</v>
-      </c>
-      <c r="I5" s="7">
-        <v>1.189579543</v>
-      </c>
-      <c r="J5" s="7">
-        <v>1.159648563</v>
-      </c>
-      <c r="K5" s="7">
-        <v>1.156311054</v>
-      </c>
-      <c r="L5" s="7">
-        <v>1.170361225</v>
-      </c>
-      <c r="M5" s="6">
-        <v>1.398143636</v>
+      <c r="L5" s="3">
+        <v>1.395511162</v>
+      </c>
+      <c r="M5" s="9">
+        <v>1.306950274</v>
+      </c>
+      <c r="N5" s="8">
+        <v>1.452914817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update benchmark and ablation files for multicore testing
</commit_message>
<xml_diff>
--- a/ablation-revised/ablation.xlsx
+++ b/ablation-revised/ablation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Adaptive</t>
   </si>
@@ -48,15 +48,6 @@
   </si>
   <si>
     <t>1 Core</t>
-  </si>
-  <si>
-    <t>2 Core</t>
-  </si>
-  <si>
-    <t>4 Core</t>
-  </si>
-  <si>
-    <t>8 Core</t>
   </si>
 </sst>
 </file>
@@ -118,34 +109,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -155,9 +143,6 @@
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -461,26 +446,26 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="44.25">
@@ -519,7 +504,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -530,169 +515,37 @@
         <v>1.046469666</v>
       </c>
       <c r="D2" s="8">
-        <v>1.220290755</v>
+        <v>1.09786521</v>
       </c>
       <c r="E2" s="3">
         <v>1.088374371</v>
       </c>
       <c r="F2" s="3">
+        <v>1.065259394</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1.081262376</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1.250514984</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.226602354</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1.220290755</v>
+      </c>
+      <c r="K2" s="3">
         <v>1.201244868</v>
       </c>
-      <c r="G2" s="3">
-        <v>1.065259394</v>
-      </c>
-      <c r="H2" s="3">
-        <v>1.226602354</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.09786521</v>
-      </c>
-      <c r="J2" s="3">
+      <c r="L2" s="3">
         <v>1.193264524</v>
       </c>
-      <c r="K2" s="3">
-        <v>1.081262376</v>
-      </c>
-      <c r="L2" s="3">
+      <c r="M2" s="4">
         <v>1.393359136</v>
-      </c>
-      <c r="M2" s="9">
-        <v>1.250514984</v>
       </c>
       <c r="N2" s="8">
         <v>1.410047258</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="7">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8">
-        <v>1.044947754</v>
-      </c>
-      <c r="D3" s="8">
-        <v>1.222614297</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1.088441801</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1.201961981</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1.063494276</v>
-      </c>
-      <c r="H3" s="3">
-        <v>1.223025188</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.097107283</v>
-      </c>
-      <c r="J3" s="3">
-        <v>1.194124163</v>
-      </c>
-      <c r="K3" s="3">
-        <v>1.080079914</v>
-      </c>
-      <c r="L3" s="3">
-        <v>1.400666465</v>
-      </c>
-      <c r="M3" s="9">
-        <v>1.258327406</v>
-      </c>
-      <c r="N3" s="8">
-        <v>1.411655629</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="7">
-        <v>1</v>
-      </c>
-      <c r="C4" s="8">
-        <v>1.048338979</v>
-      </c>
-      <c r="D4" s="8">
-        <v>1.195723665</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1.097846976</v>
-      </c>
-      <c r="F4" s="3">
-        <v>1.158447513</v>
-      </c>
-      <c r="G4" s="3">
-        <v>1.066200261</v>
-      </c>
-      <c r="H4" s="3">
-        <v>1.161759297</v>
-      </c>
-      <c r="I4" s="3">
-        <v>1.066450554</v>
-      </c>
-      <c r="J4" s="3">
-        <v>1.179059897</v>
-      </c>
-      <c r="K4" s="3">
-        <v>1.074580819</v>
-      </c>
-      <c r="L4" s="3">
-        <v>1.366567845</v>
-      </c>
-      <c r="M4" s="9">
-        <v>1.257503414</v>
-      </c>
-      <c r="N4" s="8">
-        <v>1.440002459</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="7">
-        <v>1</v>
-      </c>
-      <c r="C5" s="8">
-        <v>1.045820092</v>
-      </c>
-      <c r="D5" s="8">
-        <v>1.189579543</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1.101474491</v>
-      </c>
-      <c r="F5" s="3">
-        <v>1.159648563</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1.071425026</v>
-      </c>
-      <c r="H5" s="3">
-        <v>1.156311054</v>
-      </c>
-      <c r="I5" s="3">
-        <v>1.064313615</v>
-      </c>
-      <c r="J5" s="3">
-        <v>1.170361225</v>
-      </c>
-      <c r="K5" s="3">
-        <v>1.076043693</v>
-      </c>
-      <c r="L5" s="3">
-        <v>1.395511162</v>
-      </c>
-      <c r="M5" s="9">
-        <v>1.306950274</v>
-      </c>
-      <c r="N5" s="8">
-        <v>1.452914817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>